<commit_message>
Variable name: OBS -> OBSCRI
</commit_message>
<xml_diff>
--- a/app/config/tables/CHILDREN/Forms/CHILDREN/CHILDREN.xlsx
+++ b/app/config/tables/CHILDREN/Forms/CHILDREN/CHILDREN.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229F6F76-D617-4C04-BD8A-C018F38B8C88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986C9451-43D5-44DA-A76E-88968C5267A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -888,13 +888,13 @@
     <t>Se o MUAC for menor que 50 mm, escreva "11" &lt;/br&gt; Se não for possível medir o MUAC, escreva "999"</t>
   </si>
   <si>
-    <t>OBS</t>
-  </si>
-  <si>
     <t>&lt;i&gt; If you have any comment or observations about the child, write them here &lt;/i&gt;</t>
   </si>
   <si>
     <t>&lt;i&gt; Se você tiver algum comentário ou observação sobre a criança, escreva aqui &lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>OBSCRI</t>
   </si>
 </sst>
 </file>
@@ -1456,7 +1456,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E98" sqref="E98"/>
+      <selection pane="bottomLeft" activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2661,13 +2661,13 @@
         <v>61</v>
       </c>
       <c r="F99" t="s">
+        <v>286</v>
+      </c>
+      <c r="G99" t="s">
         <v>284</v>
       </c>
-      <c r="G99" t="s">
+      <c r="H99" t="s">
         <v>285</v>
-      </c>
-      <c r="H99" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="100" spans="2:8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3904,8 +3904,8 @@
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4441,7 +4441,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Implemented data permission filters
</commit_message>
<xml_diff>
--- a/app/config/tables/CHILDREN/Forms/CHILDREN/CHILDREN.xlsx
+++ b/app/config/tables/CHILDREN/Forms/CHILDREN/CHILDREN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11A79F7-52BE-43EC-AEC5-4C6B004F3785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235D27BB-08C2-4E5F-9189-04A8C092B1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="728" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="calculates" sheetId="7" r:id="rId5"/>
     <sheet name="prompt_types" sheetId="6" r:id="rId6"/>
     <sheet name="model" sheetId="4" r:id="rId7"/>
+    <sheet name="properties" sheetId="14" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="353">
   <si>
     <t>setting_name</t>
   </si>
@@ -1064,6 +1065,36 @@
   </si>
   <si>
     <t>Estado da criança</t>
+  </si>
+  <si>
+    <t>partition</t>
+  </si>
+  <si>
+    <t>aspect</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>locked</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>unverifiedUserCanCreate</t>
+  </si>
+  <si>
+    <t>defaultAccessOnCreation</t>
+  </si>
+  <si>
+    <t>HIDDEN</t>
   </si>
 </sst>
 </file>
@@ -1616,7 +1647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
   <dimension ref="A1:T161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
     </sheetView>
@@ -5625,4 +5656,97 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20ACF115-0936-4F5A-8A74-965B4D967D9F}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D2" t="s">
+        <v>349</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"FALSE"</f>
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="D3" t="s">
+        <v>349</v>
+      </c>
+      <c r="E3" t="str">
+        <f>"TRUE"</f>
+        <v>TRUE</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>346</v>
+      </c>
+      <c r="B4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>